<commit_message>
Finish Rice Reporting Print
</commit_message>
<xml_diff>
--- a/Templates/RicePlantingReport.xlsx
+++ b/Templates/RicePlantingReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Documents\AgRecords\AgRecords Github\AgRecords\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD87F33-DB07-43F4-8C85-EEEB526C8375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E3BB19-05C3-44BF-AE89-AD6C9EADF1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2364" yWindow="720" windowWidth="17280" windowHeight="8880" xr2:uid="{2B127761-3FE7-4873-8B24-07FACE8F897C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2B127761-3FE7-4873-8B24-07FACE8F897C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1142,7 +1142,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1180,27 +1180,6 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1216,25 +1195,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1267,6 +1228,33 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2376,8 +2364,8 @@
   </sheetPr>
   <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="80" zoomScaleNormal="40" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:F8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2562,806 +2550,866 @@
       <c r="V6" s="11"/>
     </row>
     <row r="7" spans="1:28" ht="18" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42"/>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="42"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="44" t="s">
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="31" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="18" x14ac:dyDescent="0.3">
-      <c r="A8" s="40"/>
-      <c r="B8" s="41" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="44" t="s">
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44" t="s">
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="44"/>
-      <c r="N8" s="44"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="45" t="s">
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="41" t="s">
+      <c r="Q8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="42"/>
-      <c r="U8" s="43"/>
-      <c r="V8" s="44"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="30"/>
+      <c r="V8" s="31"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
-      <c r="B9" s="45" t="s">
+      <c r="A9" s="27"/>
+      <c r="B9" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="45" t="s">
+      <c r="H9" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="45" t="s">
+      <c r="I9" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="45" t="s">
+      <c r="J9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="45" t="s">
+      <c r="K9" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="45" t="s">
+      <c r="L9" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="45" t="s">
+      <c r="M9" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="N9" s="45" t="s">
+      <c r="N9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="O9" s="45" t="s">
+      <c r="O9" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="45" t="s">
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="R9" s="45" t="s">
+      <c r="R9" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="S9" s="45" t="s">
+      <c r="S9" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="T9" s="45" t="s">
+      <c r="T9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="U9" s="39" t="s">
+      <c r="U9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="V9" s="44"/>
+      <c r="V9" s="31"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="45"/>
-      <c r="R10" s="45"/>
-      <c r="S10" s="45"/>
-      <c r="T10" s="45"/>
-      <c r="U10" s="40"/>
-      <c r="V10" s="44"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="31"/>
     </row>
     <row r="11" spans="1:28" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A11" s="40"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="45"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="44"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="31"/>
       <c r="AA11" s="13"/>
     </row>
     <row r="12" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="17"/>
-      <c r="U12" s="17"/>
-      <c r="V12" s="22"/>
-      <c r="AA12" s="23">
+      <c r="B12" s="35"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="15"/>
+      <c r="AA12" s="16">
         <v>31.25</v>
       </c>
-      <c r="AB12" s="24"/>
+      <c r="AB12" s="17"/>
     </row>
     <row r="13" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="17"/>
-      <c r="V13" s="25"/>
-      <c r="AA13" s="26">
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="18"/>
+      <c r="AA13" s="19">
         <v>41.5</v>
       </c>
-      <c r="AB13" s="24"/>
+      <c r="AB13" s="17"/>
     </row>
     <row r="14" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="25"/>
-      <c r="AA14" s="26" t="s">
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="18"/>
+      <c r="AA14" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AB14" s="24"/>
+      <c r="AB14" s="17"/>
     </row>
     <row r="15" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="17"/>
-      <c r="V15" s="31"/>
-      <c r="AA15" s="26" t="s">
+      <c r="B15" s="39"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="20"/>
+      <c r="AA15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AB15" s="24"/>
+      <c r="AB15" s="17"/>
     </row>
     <row r="16" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="17"/>
-      <c r="U16" s="17"/>
-      <c r="V16" s="22"/>
-      <c r="AA16" s="26">
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="37"/>
+      <c r="V16" s="15"/>
+      <c r="AA16" s="19">
         <v>93.7</v>
       </c>
-      <c r="AB16" s="24"/>
+      <c r="AB16" s="17"/>
     </row>
     <row r="17" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="17"/>
-      <c r="V17" s="22"/>
-      <c r="AA17" s="26">
+      <c r="B17" s="35"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="15"/>
+      <c r="AA17" s="19">
         <v>85.55</v>
       </c>
-      <c r="AB17" s="24"/>
+      <c r="AB17" s="17"/>
     </row>
     <row r="18" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="17"/>
-      <c r="U18" s="17"/>
-      <c r="V18" s="25"/>
-      <c r="AA18" s="26" t="s">
+      <c r="B18" s="35"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="37"/>
+      <c r="U18" s="37"/>
+      <c r="V18" s="18"/>
+      <c r="AA18" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AB18" s="24"/>
+      <c r="AB18" s="17"/>
     </row>
     <row r="19" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
-      <c r="U19" s="17"/>
-      <c r="V19" s="25"/>
-      <c r="AA19" s="26">
+      <c r="B19" s="35"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="18"/>
+      <c r="AA19" s="19">
         <v>17.059999999999999</v>
       </c>
-      <c r="AB19" s="24"/>
+      <c r="AB19" s="17"/>
     </row>
     <row r="20" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
-      <c r="U20" s="17"/>
-      <c r="V20" s="31"/>
-      <c r="AA20" s="26" t="s">
+      <c r="B20" s="39"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="37"/>
+      <c r="U20" s="37"/>
+      <c r="V20" s="20"/>
+      <c r="AA20" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AB20" s="24"/>
+      <c r="AB20" s="17"/>
     </row>
     <row r="21" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17"/>
-      <c r="U21" s="17"/>
-      <c r="V21" s="22"/>
-      <c r="AA21" s="26" t="s">
+      <c r="B21" s="35"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="37"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="15"/>
+      <c r="AA21" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AB21" s="24"/>
+      <c r="AB21" s="17"/>
     </row>
     <row r="22" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
-      <c r="U22" s="17"/>
-      <c r="V22" s="22"/>
-      <c r="AA22" s="26">
+      <c r="B22" s="35"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="37"/>
+      <c r="V22" s="15"/>
+      <c r="AA22" s="19">
         <v>75.510000000000005</v>
       </c>
-      <c r="AB22" s="24"/>
+      <c r="AB22" s="17"/>
     </row>
     <row r="23" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
-      <c r="U23" s="17"/>
-      <c r="V23" s="25"/>
-      <c r="AA23" s="26">
+      <c r="B23" s="35"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="37"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="37"/>
+      <c r="U23" s="37"/>
+      <c r="V23" s="18"/>
+      <c r="AA23" s="19">
         <v>72.78</v>
       </c>
-      <c r="AB23" s="24"/>
+      <c r="AB23" s="17"/>
     </row>
     <row r="24" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="21"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17"/>
-      <c r="U24" s="17"/>
-      <c r="V24" s="25"/>
-      <c r="AA24" s="26">
+      <c r="B24" s="35"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="37"/>
+      <c r="U24" s="37"/>
+      <c r="V24" s="18"/>
+      <c r="AA24" s="19">
         <v>112.75</v>
       </c>
-      <c r="AB24" s="24"/>
+      <c r="AB24" s="17"/>
     </row>
     <row r="25" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="21"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
-      <c r="U25" s="17"/>
-      <c r="V25" s="31"/>
-      <c r="AA25" s="26">
+      <c r="B25" s="39"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="20"/>
+      <c r="AA25" s="19">
         <v>63.7</v>
       </c>
-      <c r="AB25" s="24"/>
+      <c r="AB25" s="17"/>
     </row>
     <row r="26" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="17"/>
-      <c r="S26" s="17"/>
-      <c r="T26" s="17"/>
-      <c r="U26" s="17"/>
-      <c r="V26" s="22"/>
-      <c r="AA26" s="26">
+      <c r="B26" s="35"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="37"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="37"/>
+      <c r="U26" s="37"/>
+      <c r="V26" s="15"/>
+      <c r="AA26" s="19">
         <v>195.85</v>
       </c>
-      <c r="AB26" s="24"/>
+      <c r="AB26" s="17"/>
     </row>
     <row r="27" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="21"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
-      <c r="U27" s="17"/>
-      <c r="V27" s="22"/>
-      <c r="AA27" s="26">
+      <c r="B27" s="35"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="37"/>
+      <c r="U27" s="37"/>
+      <c r="V27" s="15"/>
+      <c r="AA27" s="19">
         <v>162.80000000000001</v>
       </c>
-      <c r="AB27" s="24"/>
+      <c r="AB27" s="17"/>
     </row>
     <row r="28" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="21"/>
-      <c r="R28" s="17"/>
-      <c r="S28" s="17"/>
-      <c r="T28" s="17"/>
-      <c r="U28" s="17"/>
-      <c r="V28" s="25"/>
-      <c r="AA28" s="26">
+      <c r="B28" s="35"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="37"/>
+      <c r="U28" s="37"/>
+      <c r="V28" s="18"/>
+      <c r="AA28" s="19">
         <v>227.4</v>
       </c>
-      <c r="AB28" s="24"/>
+      <c r="AB28" s="17"/>
     </row>
     <row r="29" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="19"/>
-      <c r="P29" s="20"/>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="17"/>
-      <c r="S29" s="17"/>
-      <c r="T29" s="17"/>
-      <c r="U29" s="17"/>
-      <c r="V29" s="25"/>
-      <c r="AA29" s="26" t="s">
+      <c r="B29" s="35"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="37"/>
+      <c r="R29" s="37"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="37"/>
+      <c r="U29" s="37"/>
+      <c r="V29" s="18"/>
+      <c r="AA29" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AB29" s="24"/>
+      <c r="AB29" s="17"/>
     </row>
     <row r="30" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="21"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="17"/>
-      <c r="T30" s="17"/>
-      <c r="U30" s="17"/>
-      <c r="V30" s="31"/>
-      <c r="AA30" s="26">
+      <c r="B30" s="39"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="37"/>
+      <c r="Q30" s="37"/>
+      <c r="R30" s="37"/>
+      <c r="S30" s="37"/>
+      <c r="T30" s="37"/>
+      <c r="U30" s="37"/>
+      <c r="V30" s="20"/>
+      <c r="AA30" s="19">
         <v>197.8</v>
       </c>
-      <c r="AB30" s="24"/>
+      <c r="AB30" s="17"/>
     </row>
     <row r="31" spans="1:28" ht="45.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
-      <c r="T31" s="17"/>
-      <c r="U31" s="17"/>
-      <c r="V31" s="22"/>
-      <c r="AA31" s="26">
+      <c r="B31" s="35"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="38"/>
+      <c r="P31" s="37"/>
+      <c r="Q31" s="37"/>
+      <c r="R31" s="37"/>
+      <c r="S31" s="37"/>
+      <c r="T31" s="37"/>
+      <c r="U31" s="37"/>
+      <c r="V31" s="15"/>
+      <c r="AA31" s="19">
         <v>168.56</v>
       </c>
-      <c r="AB31" s="24"/>
+      <c r="AB31" s="17"/>
     </row>
     <row r="32" spans="1:28" ht="45.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="32"/>
-      <c r="N32" s="32"/>
-      <c r="O32" s="32"/>
-      <c r="P32" s="33"/>
-      <c r="Q32" s="32"/>
-      <c r="R32" s="33"/>
-      <c r="S32" s="33"/>
-      <c r="T32" s="33"/>
-      <c r="U32" s="33"/>
-      <c r="V32" s="22"/>
-      <c r="AA32" s="34"/>
+      <c r="B32" s="34">
+        <f>SUM(B12:B31)</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="34">
+        <f t="shared" ref="C32:U32" si="0">SUM(C12:C31)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U32" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V32" s="15"/>
+      <c r="AA32" s="21"/>
     </row>
     <row r="33" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="11"/>
@@ -3388,25 +3436,25 @@
       <c r="V33" s="11"/>
     </row>
     <row r="34" spans="1:22" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="35"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="35" t="s">
+      <c r="B34" s="22"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="I34" s="35"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="35"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="35"/>
-      <c r="P34" s="35"/>
-      <c r="Q34" s="37"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="24"/>
       <c r="R34" s="11"/>
       <c r="S34" s="11"/>
       <c r="T34" s="11"/>
@@ -3414,25 +3462,25 @@
       <c r="V34" s="11"/>
     </row>
     <row r="35" spans="1:22" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A35" s="35"/>
-      <c r="B35" s="38" t="s">
+      <c r="A35" s="22"/>
+      <c r="B35" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="38" t="s">
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="J35" s="35"/>
-      <c r="K35" s="35"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="38"/>
-      <c r="O35" s="35"/>
-      <c r="P35" s="35"/>
-      <c r="Q35" s="37"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="24"/>
       <c r="R35" s="11"/>
       <c r="S35" s="11"/>
       <c r="T35" s="11"/>
@@ -3440,25 +3488,25 @@
       <c r="V35" s="11"/>
     </row>
     <row r="36" spans="1:22" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A36" s="35"/>
-      <c r="B36" s="35" t="s">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="35" t="s">
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="J36" s="35"/>
-      <c r="K36" s="35"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="35"/>
-      <c r="N36" s="35"/>
-      <c r="O36" s="35"/>
-      <c r="P36" s="35"/>
-      <c r="Q36" s="37"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="24"/>
       <c r="R36" s="11"/>
       <c r="S36" s="11"/>
       <c r="T36" s="11"/>

</xml_diff>